<commit_message>
added originality rate section in the main notebook
</commit_message>
<xml_diff>
--- a/pivot_table.xlsx
+++ b/pivot_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,70 +506,60 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>GR</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>HU</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>KR</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>KR</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>NL</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>PL</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>PL</t>
+          <t>RU</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>TW</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>TR</t>
+          <t>US</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>TW</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>WO</t>
         </is>
@@ -578,7 +568,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>AU</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -630,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -654,107 +644,95 @@
         <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>EP</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>290</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
         <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
         <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>9</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>58</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>DK</t>
+          <t>GB</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -830,19 +808,13 @@
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>EP</t>
+          <t>TW</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -858,7 +830,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -870,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
@@ -906,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
         <v>0</v>
@@ -918,19 +890,13 @@
         <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>WO</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -940,19 +906,19 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -961,13 +927,13 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -985,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="S6" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T6" t="n">
         <v>0</v>
@@ -997,28 +963,22 @@
         <v>0</v>
       </c>
       <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z6" t="n">
         <v>1</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>KR</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1034,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1046,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -1058,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
@@ -1070,10 +1030,10 @@
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -1088,19 +1048,13 @@
         <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -1119,10 +1073,10 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -1134,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -1146,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
@@ -1158,13 +1112,13 @@
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="S8" t="n">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="T8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
@@ -1176,459 +1130,177 @@
         <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y8" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Z8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>4</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>KR</t>
+          <t>US</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>0</v>
       </c>
       <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>46</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
         <v>1</v>
       </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" t="n">
+        <v>9</v>
+      </c>
+      <c r="K9" t="n">
+        <v>4</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>16</v>
+      </c>
+      <c r="S9" t="n">
+        <v>13</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y9" t="n">
         <v>20</v>
       </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" t="n">
-        <v>9</v>
-      </c>
-      <c r="T9" t="n">
-        <v>15</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" t="n">
-        <v>0</v>
-      </c>
-      <c r="W9" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>0</v>
-      </c>
       <c r="Z9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>13</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>CN</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F10" t="n">
+        <v>225</v>
+      </c>
+      <c r="G10" t="n">
         <v>1</v>
       </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="T10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Y10" t="n">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="Z10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>TW</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S11" t="n">
-        <v>0</v>
-      </c>
-      <c r="T11" t="n">
-        <v>0</v>
-      </c>
-      <c r="U11" t="n">
-        <v>0</v>
-      </c>
-      <c r="V11" t="n">
-        <v>0</v>
-      </c>
-      <c r="W11" t="n">
-        <v>0</v>
-      </c>
-      <c r="X11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>5</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4</v>
-      </c>
-      <c r="F12" t="n">
-        <v>42</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>6</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>9</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>2</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0</v>
-      </c>
-      <c r="S12" t="n">
-        <v>23</v>
-      </c>
-      <c r="T12" t="n">
-        <v>9</v>
-      </c>
-      <c r="U12" t="n">
-        <v>1</v>
-      </c>
-      <c r="V12" t="n">
-        <v>0</v>
-      </c>
-      <c r="W12" t="n">
-        <v>0</v>
-      </c>
-      <c r="X12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>55</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>WO</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>10</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>2</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0</v>
-      </c>
-      <c r="S13" t="n">
-        <v>0</v>
-      </c>
-      <c r="T13" t="n">
-        <v>5</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0</v>
-      </c>
-      <c r="V13" t="n">
-        <v>0</v>
-      </c>
-      <c r="W13" t="n">
-        <v>0</v>
-      </c>
-      <c r="X13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>